<commit_message>
requests to omdbAPI for more information
</commit_message>
<xml_diff>
--- a/Expenses03.xlsx
+++ b/Expenses03.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Title</t>
   </si>
@@ -25,55 +25,37 @@
     <t>Director</t>
   </si>
   <si>
-    <t>Fantastic Beasts</t>
-  </si>
-  <si>
-    <t>Manchester by the Sea</t>
-  </si>
-  <si>
-    <t>Deadpool 2</t>
-  </si>
-  <si>
-    <t>Aquaman</t>
-  </si>
-  <si>
-    <t>Rogue One: A Star Wars Story</t>
-  </si>
-  <si>
-    <t>Inner City</t>
-  </si>
-  <si>
-    <t>Triple Frontier</t>
-  </si>
-  <si>
-    <t>Grasshopper Jungle</t>
-  </si>
-  <si>
-    <t>Mortal Engines</t>
-  </si>
-  <si>
-    <t>The Untamed</t>
-  </si>
-  <si>
-    <t>Beatriz at Dinner</t>
-  </si>
-  <si>
-    <t>Beauty and the Beast</t>
-  </si>
-  <si>
-    <t>Get Out</t>
-  </si>
-  <si>
-    <t>Infinity Baby</t>
-  </si>
-  <si>
-    <t>Mission Control: The Unsung Heroes of Apollo</t>
-  </si>
-  <si>
-    <t>Born in China</t>
-  </si>
-  <si>
-    <t>Leaning Into the Wind</t>
+    <t>Plot</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>7.8</t>
+  </si>
+  <si>
+    <t>Achero Mañas</t>
+  </si>
+  <si>
+    <t>Impelled by a spirit which still preserves a patina of idealism, Alfredo arrives in Madrid intent on creating "a performance which is freer, straight from the heart, capable of making ...</t>
+  </si>
+  <si>
+    <t>Outlaw King</t>
+  </si>
+  <si>
+    <t>Not found</t>
+  </si>
+  <si>
+    <t>The Nun</t>
+  </si>
+  <si>
+    <t>4.0</t>
+  </si>
+  <si>
+    <t>Luis de la Madrid</t>
+  </si>
+  <si>
+    <t>A group of teenage girls are terrorized by Sister Ursula, a nun that believes she must rid the world of all sin. After Sister Ursula mysteriously disappears, the Catholic school is shut ...</t>
   </si>
 </sst>
 </file>
@@ -405,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -414,7 +396,7 @@
     <col min="1" max="1" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,90 +406,50 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
+      <c r="D4" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added role parser, cleaned up and commented code
</commit_message>
<xml_diff>
--- a/Expenses03.xlsx
+++ b/Expenses03.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Title</t>
   </si>
@@ -28,34 +28,28 @@
     <t>Plot</t>
   </si>
   <si>
-    <t>November</t>
+    <t>Someone Else</t>
+  </si>
+  <si>
+    <t>5.9</t>
+  </si>
+  <si>
+    <t>Col Spector</t>
+  </si>
+  <si>
+    <t>Cameo Appearance of Neville Bardoliwalla as Freddie Mercury.</t>
+  </si>
+  <si>
+    <t>A Star Is Born</t>
   </si>
   <si>
     <t>7.8</t>
   </si>
   <si>
-    <t>Achero Mañas</t>
-  </si>
-  <si>
-    <t>Impelled by a spirit which still preserves a patina of idealism, Alfredo arrives in Madrid intent on creating "a performance which is freer, straight from the heart, capable of making ...</t>
-  </si>
-  <si>
-    <t>Outlaw King</t>
-  </si>
-  <si>
-    <t>Not found</t>
-  </si>
-  <si>
-    <t>The Nun</t>
-  </si>
-  <si>
-    <t>4.0</t>
-  </si>
-  <si>
-    <t>Luis de la Madrid</t>
-  </si>
-  <si>
-    <t>A group of teenage girls are terrorized by Sister Ursula, a nun that believes she must rid the world of all sin. After Sister Ursula mysteriously disappears, the Catholic school is shut ...</t>
+    <t>George Cukor</t>
+  </si>
+  <si>
+    <t>A film star helps a young singer and actress find fame, even as age and alcoholism send his own career on a downward spiral.</t>
   </si>
 </sst>
 </file>
@@ -387,7 +381,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -432,24 +426,10 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>